<commit_message>
update and change code
</commit_message>
<xml_diff>
--- a/todolist.xlsx
+++ b/todolist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Item</t>
   </si>
@@ -25,16 +25,7 @@
     <t>ali</t>
   </si>
   <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>4</t>
+    <t>high</t>
   </si>
 </sst>
 </file>
@@ -352,7 +343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="B5" sqref="B5"/>
@@ -379,30 +370,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
add or 3000 to PORT
</commit_message>
<xml_diff>
--- a/todolist.xlsx
+++ b/todolist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Item</t>
   </si>
@@ -22,10 +22,19 @@
     <t>Priority</t>
   </si>
   <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
     <t>ali</t>
   </si>
   <si>
-    <t>high</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>w</t>
   </si>
 </sst>
 </file>
@@ -343,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="B5" sqref="B5"/>
@@ -370,6 +379,30 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>